<commit_message>
Done process export excel
</commit_message>
<xml_diff>
--- a/template-equivalent-tables.xlsx
+++ b/template-equivalent-tables.xlsx
@@ -13,9 +13,10 @@
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
-    <sheet name="config" sheetId="2" r:id="rId2"/>
-    <sheet name="data" sheetId="3" r:id="rId3"/>
-    <sheet name="Report (2)" sheetId="4" r:id="rId4"/>
+    <sheet name="Report (3)" sheetId="5" r:id="rId2"/>
+    <sheet name="Report (4)" sheetId="6" r:id="rId3"/>
+    <sheet name="config" sheetId="2" r:id="rId4"/>
+    <sheet name="data" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913" iterate="1"/>
   <extLst>
@@ -82,7 +83,32 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0" shapeId="0">
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>AdonisGM:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+0: Không có merge cell trong report
+1: Có merge cell trong report</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -106,7 +132,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -130,7 +156,155 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>AdonisGM:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Các cột thông tin của bảng,
+Nếu là bảng cuối cùng không điền tên cột vì sẽ lấy all
+Nếu có nhiều cột thì ngăn cách bằng dấu ",". VD: "ABC,EDO"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>AdonisGM:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Toạ độ bắt đầu của bảng</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>AdonisGM:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Toạ độ kết thúc của bảng</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>AdonisGM:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Các cột thông tin của bảng,
+Nếu là bảng cuối cùng không điền tên cột vì sẽ lấy all
+Nếu có nhiều cột thì ngăn cách bằng dấu ",". VD: "ABC,EDO"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B21" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>AdonisGM:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Toạ độ bắt đầu của bảng</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C21" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>AdonisGM:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Toạ độ kết thúc của bảng</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -161,7 +335,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1897" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1938" uniqueCount="182">
   <si>
     <t>range_1</t>
   </si>
@@ -686,6 +860,27 @@
   </si>
   <si>
     <t>K16</t>
+  </si>
+  <si>
+    <t>&lt;#table.SHARE_FREE&gt;</t>
+  </si>
+  <si>
+    <t>&lt;#table.SHARE_BLOCK&gt;</t>
+  </si>
+  <si>
+    <t>sheet_0</t>
+  </si>
+  <si>
+    <t>sheet_1</t>
+  </si>
+  <si>
+    <t>sheet_2</t>
+  </si>
+  <si>
+    <t>isMultipleSheet</t>
+  </si>
+  <si>
+    <t>&lt;#table.SHARE_CODE&gt; - &lt;#table.SHARE_CODE&gt; - &lt;#table.SHARE_CODE&gt;</t>
   </si>
 </sst>
 </file>
@@ -768,7 +963,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -841,20 +1036,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1000,11 +1183,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1092,9 +1284,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="8" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1125,41 +1314,26 @@
     <xf numFmtId="49" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="8" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="8" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1186,6 +1360,15 @@
     <xf numFmtId="3" fontId="8" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1201,28 +1384,10 @@
     <xf numFmtId="3" fontId="8" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="8" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="8" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="8" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1568,10 +1733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S29"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AC17" sqref="AC17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.88671875" defaultRowHeight="15"/>
@@ -1579,75 +1744,72 @@
     <col min="2" max="3" width="3.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:16">
       <c r="A1" s="39" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:16">
       <c r="A2" s="39"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:16">
       <c r="A3" s="40" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:16">
       <c r="A5" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64" t="s">
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="64"/>
-      <c r="J5" s="64"/>
-      <c r="K5" s="64" t="s">
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="L5" s="64"/>
-      <c r="M5" s="64"/>
-      <c r="N5" s="64"/>
-      <c r="O5" s="64"/>
-      <c r="P5" s="64"/>
-    </row>
-    <row r="6" spans="1:19">
+      <c r="L5" s="58"/>
+      <c r="M5" s="58"/>
+      <c r="N5" s="58"/>
+      <c r="O5" s="58"/>
+      <c r="P5" s="58"/>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="67" t="s">
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="59" t="s">
         <v>74</v>
       </c>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="69"/>
-      <c r="K6" s="67" t="s">
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="L6" s="68"/>
-      <c r="M6" s="68"/>
-      <c r="N6" s="68"/>
-      <c r="O6" s="68"/>
-      <c r="P6" s="69"/>
-      <c r="Q6" s="58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19">
+      <c r="L6" s="60"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="60"/>
+      <c r="O6" s="60"/>
+      <c r="P6" s="61"/>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" s="20"/>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
@@ -1664,151 +1826,129 @@
       <c r="N7" s="23"/>
       <c r="O7" s="23"/>
       <c r="P7" s="24"/>
-      <c r="Q7" s="58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19">
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" s="25"/>
       <c r="B8" s="21"/>
       <c r="C8" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="61" t="s">
+      <c r="D8" s="67" t="s">
         <v>63</v>
       </c>
-      <c r="E8" s="62"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="64" t="s">
+      <c r="E8" s="68"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="58" t="s">
         <v>64</v>
       </c>
-      <c r="H8" s="64"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="64"/>
-      <c r="K8" s="64"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="58"/>
       <c r="L8" s="23"/>
       <c r="M8" s="23"/>
       <c r="N8" s="23"/>
       <c r="O8" s="23"/>
       <c r="P8" s="26"/>
-      <c r="Q8" s="58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19">
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" s="25"/>
       <c r="B9" s="21"/>
       <c r="C9" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="71" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9" s="72"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="74" t="s">
+      <c r="D9" s="63" t="s">
+        <v>181</v>
+      </c>
+      <c r="E9" s="64"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="H9" s="74"/>
-      <c r="I9" s="74"/>
-      <c r="J9" s="74"/>
-      <c r="K9" s="74"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="66"/>
       <c r="L9" s="23"/>
       <c r="M9" s="23"/>
       <c r="N9" s="23"/>
       <c r="O9" s="23"/>
       <c r="P9" s="26"/>
-      <c r="Q9">
-        <v>1</v>
-      </c>
-      <c r="R9" s="60"/>
-    </row>
-    <row r="10" spans="1:19">
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" s="25"/>
       <c r="B10" s="21"/>
       <c r="C10" s="19"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="46"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="45"/>
       <c r="K10" s="24"/>
       <c r="L10" s="23"/>
       <c r="M10" s="23"/>
       <c r="N10" s="23"/>
       <c r="O10" s="23"/>
       <c r="P10" s="26"/>
-      <c r="Q10">
-        <v>1</v>
-      </c>
-      <c r="R10" s="60"/>
-    </row>
-    <row r="11" spans="1:19">
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11" s="25"/>
       <c r="B11" s="21"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="51" t="s">
+      <c r="C11" s="48"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="75" t="s">
+      <c r="F11" s="70" t="s">
         <v>95</v>
       </c>
-      <c r="G11" s="75"/>
-      <c r="H11" s="76" t="s">
+      <c r="G11" s="70"/>
+      <c r="H11" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="I11" s="76"/>
-      <c r="J11" s="76"/>
+      <c r="I11" s="71"/>
+      <c r="J11" s="71"/>
       <c r="K11" s="26"/>
       <c r="L11" s="23"/>
       <c r="M11" s="23"/>
       <c r="N11" s="23"/>
       <c r="O11" s="23"/>
       <c r="P11" s="26"/>
-      <c r="Q11">
-        <v>1</v>
-      </c>
-      <c r="R11" s="60"/>
-    </row>
-    <row r="12" spans="1:19">
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" s="25"/>
       <c r="B12" s="21"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="42"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="41"/>
       <c r="E12" s="38"/>
-      <c r="F12" s="71" t="s">
+      <c r="F12" s="63" t="s">
         <v>96</v>
       </c>
-      <c r="G12" s="73"/>
-      <c r="H12" s="77" t="s">
+      <c r="G12" s="65"/>
+      <c r="H12" s="72" t="s">
         <v>97</v>
       </c>
-      <c r="I12" s="78"/>
-      <c r="J12" s="79"/>
+      <c r="I12" s="73"/>
+      <c r="J12" s="74"/>
       <c r="K12" s="26"/>
       <c r="L12" s="23"/>
       <c r="M12" s="23"/>
       <c r="N12" s="23"/>
       <c r="O12" s="23"/>
       <c r="P12" s="26"/>
-      <c r="Q12">
-        <v>1</v>
-      </c>
-      <c r="S12" s="59"/>
-    </row>
-    <row r="13" spans="1:19">
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" s="25"/>
       <c r="B13" s="21"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
       <c r="J13" s="22"/>
       <c r="K13" s="26"/>
       <c r="L13" s="23"/>
@@ -1816,75 +1956,63 @@
       <c r="N13" s="23"/>
       <c r="O13" s="23"/>
       <c r="P13" s="26"/>
-      <c r="Q13">
-        <v>1</v>
-      </c>
-      <c r="R13" s="60"/>
-    </row>
-    <row r="14" spans="1:19">
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" s="25"/>
       <c r="B14" s="21"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="51" t="s">
+      <c r="C14" s="48"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="75" t="s">
+      <c r="F14" s="70" t="s">
         <v>95</v>
       </c>
-      <c r="G14" s="75"/>
-      <c r="H14" s="76" t="s">
+      <c r="G14" s="70"/>
+      <c r="H14" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="I14" s="76"/>
-      <c r="J14" s="76"/>
+      <c r="I14" s="71"/>
+      <c r="J14" s="71"/>
       <c r="K14" s="26"/>
       <c r="L14" s="23"/>
       <c r="M14" s="23"/>
       <c r="N14" s="23"/>
       <c r="O14" s="23"/>
       <c r="P14" s="26"/>
-      <c r="Q14">
-        <v>1</v>
-      </c>
-      <c r="R14" s="60"/>
-    </row>
-    <row r="15" spans="1:19">
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" s="25"/>
       <c r="B15" s="21"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="42"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="41"/>
       <c r="E15" s="38"/>
-      <c r="F15" s="71" t="s">
-        <v>96</v>
-      </c>
-      <c r="G15" s="73"/>
-      <c r="H15" s="77" t="s">
-        <v>97</v>
-      </c>
-      <c r="I15" s="78"/>
-      <c r="J15" s="79"/>
+      <c r="F15" s="63" t="s">
+        <v>175</v>
+      </c>
+      <c r="G15" s="65"/>
+      <c r="H15" s="72" t="s">
+        <v>176</v>
+      </c>
+      <c r="I15" s="73"/>
+      <c r="J15" s="74"/>
       <c r="K15" s="26"/>
       <c r="L15" s="23"/>
       <c r="M15" s="23"/>
       <c r="N15" s="23"/>
       <c r="O15" s="23"/>
       <c r="P15" s="26"/>
-      <c r="Q15">
-        <v>1</v>
-      </c>
-      <c r="S15" s="59"/>
-    </row>
-    <row r="16" spans="1:19">
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16" s="25"/>
       <c r="B16" s="21"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="48"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
       <c r="J16" s="34"/>
       <c r="K16" s="36"/>
       <c r="L16" s="23"/>
@@ -1892,12 +2020,8 @@
       <c r="N16" s="23"/>
       <c r="O16" s="23"/>
       <c r="P16" s="26"/>
-      <c r="Q16">
-        <v>1</v>
-      </c>
-      <c r="R16" s="60"/>
-    </row>
-    <row r="17" spans="1:19">
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17" s="25"/>
       <c r="B17" s="21"/>
       <c r="C17" s="21"/>
@@ -1914,11 +2038,8 @@
       <c r="N17" s="23"/>
       <c r="O17" s="23"/>
       <c r="P17" s="26"/>
-      <c r="Q17" s="58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19">
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18" s="25"/>
       <c r="B18" s="21"/>
       <c r="C18" s="29"/>
@@ -1927,25 +2048,22 @@
       <c r="F18" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="64" t="s">
+      <c r="G18" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="H18" s="64"/>
-      <c r="I18" s="64"/>
-      <c r="J18" s="64" t="s">
+      <c r="H18" s="58"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="K18" s="64"/>
-      <c r="L18" s="64"/>
+      <c r="K18" s="58"/>
+      <c r="L18" s="58"/>
       <c r="M18" s="23"/>
       <c r="N18" s="23"/>
       <c r="O18" s="23"/>
       <c r="P18" s="26"/>
-      <c r="Q18" s="58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19">
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" s="25"/>
       <c r="B19" s="21"/>
       <c r="C19" s="30"/>
@@ -1954,85 +2072,73 @@
       <c r="F19" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="G19" s="70" t="s">
+      <c r="G19" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="H19" s="70"/>
-      <c r="I19" s="70"/>
-      <c r="J19" s="74" t="s">
+      <c r="H19" s="62"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="K19" s="74"/>
-      <c r="L19" s="74"/>
+      <c r="K19" s="66"/>
+      <c r="L19" s="66"/>
       <c r="M19" s="22"/>
       <c r="N19" s="22"/>
       <c r="O19" s="22"/>
       <c r="P19" s="26"/>
-      <c r="Q19">
-        <v>1</v>
-      </c>
-      <c r="R19" s="60"/>
-    </row>
-    <row r="20" spans="1:19">
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" s="25"/>
       <c r="B20" s="21"/>
       <c r="C20" s="30"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
-      <c r="F20" s="54"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="64" t="s">
+      <c r="F20" s="52"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="I20" s="64"/>
-      <c r="J20" s="64" t="s">
+      <c r="I20" s="58"/>
+      <c r="J20" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="K20" s="64"/>
-      <c r="L20" s="64"/>
+      <c r="K20" s="58"/>
+      <c r="L20" s="58"/>
       <c r="M20" s="22"/>
       <c r="N20" s="22"/>
       <c r="O20" s="22"/>
       <c r="P20" s="26"/>
-      <c r="Q20">
-        <v>1</v>
-      </c>
-      <c r="R20" s="60"/>
-    </row>
-    <row r="21" spans="1:19">
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" s="25"/>
       <c r="B21" s="21"/>
       <c r="C21" s="30"/>
       <c r="D21" s="22"/>
       <c r="E21" s="22"/>
       <c r="F21" s="55"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="80" t="s">
+      <c r="G21" s="56"/>
+      <c r="H21" s="75" t="s">
         <v>171</v>
       </c>
-      <c r="I21" s="81"/>
-      <c r="J21" s="74" t="s">
+      <c r="I21" s="76"/>
+      <c r="J21" s="66" t="s">
         <v>169</v>
       </c>
-      <c r="K21" s="74"/>
-      <c r="L21" s="74"/>
+      <c r="K21" s="66"/>
+      <c r="L21" s="66"/>
       <c r="M21" s="22"/>
       <c r="N21" s="22"/>
       <c r="O21" s="22"/>
       <c r="P21" s="26"/>
-      <c r="Q21">
-        <v>1</v>
-      </c>
-      <c r="S21" s="59"/>
-    </row>
-    <row r="22" spans="1:19">
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22" s="31"/>
       <c r="B22" s="32"/>
       <c r="C22" s="33"/>
       <c r="D22" s="34"/>
       <c r="E22" s="34"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
       <c r="H22" s="35"/>
       <c r="I22" s="35"/>
       <c r="J22" s="35"/>
@@ -2042,91 +2148,30 @@
       <c r="N22" s="34"/>
       <c r="O22" s="34"/>
       <c r="P22" s="36"/>
-      <c r="Q22" s="58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19">
-      <c r="A23" s="28"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="56"/>
-      <c r="I23" s="56"/>
-      <c r="J23" s="56"/>
-      <c r="K23" s="56"/>
-      <c r="L23" s="56"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="22"/>
-    </row>
-    <row r="24" spans="1:19">
-      <c r="A24" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" s="61" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="62"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="61" t="s">
-        <v>64</v>
-      </c>
-      <c r="F24" s="62"/>
-      <c r="G24" s="62"/>
-      <c r="H24" s="62"/>
-      <c r="I24" s="63"/>
-      <c r="J24" s="56"/>
-      <c r="K24" s="56"/>
-      <c r="L24" s="56"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="22"/>
-      <c r="O24" s="22"/>
-      <c r="P24" s="22"/>
-    </row>
-    <row r="25" spans="1:19">
-      <c r="A25" s="57"/>
-      <c r="B25" s="85"/>
-      <c r="C25" s="86"/>
-      <c r="D25" s="87"/>
-      <c r="E25" s="82"/>
-      <c r="F25" s="83"/>
-      <c r="G25" s="83"/>
-      <c r="H25" s="83"/>
-      <c r="I25" s="84"/>
-      <c r="J25" s="56"/>
-      <c r="K25" s="56"/>
-      <c r="L25" s="56"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="22"/>
-      <c r="O25" s="22"/>
-      <c r="P25" s="22"/>
-    </row>
-    <row r="26" spans="1:19">
-      <c r="A26" s="17"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="17"/>
-    </row>
-    <row r="27" spans="1:19">
-      <c r="A27" s="39" t="s">
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" s="17"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="17"/>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="39" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:19">
-      <c r="A28" s="39"/>
-    </row>
-    <row r="29" spans="1:19">
-      <c r="A29" s="39" t="s">
+    <row r="25" spans="1:16">
+      <c r="A25" s="39"/>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" s="39" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="26">
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="F12:G12"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="H14:J14"/>
     <mergeCell ref="J21:L21"/>
@@ -2135,16 +2180,6 @@
     <mergeCell ref="H15:J15"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="J20:L20"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="B25:D25"/>
     <mergeCell ref="K5:P5"/>
     <mergeCell ref="K6:P6"/>
     <mergeCell ref="F6:J6"/>
@@ -2157,6 +2192,10 @@
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="F5:J5"/>
     <mergeCell ref="D8:F8"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:J11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -2164,11 +2203,953 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P26"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.88671875" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="3" width="3.88671875" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="39"/>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58" t="s">
+        <v>62</v>
+      </c>
+      <c r="L5" s="58"/>
+      <c r="M5" s="58"/>
+      <c r="N5" s="58"/>
+      <c r="O5" s="58"/>
+      <c r="P5" s="58"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="59" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="59" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="L6" s="60"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="60"/>
+      <c r="O6" s="60"/>
+      <c r="P6" s="61"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="20"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="24"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="25"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="67" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="68"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="58" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="58"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="26"/>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="25"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="64"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="66" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" s="66"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="66"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="26"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="25"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="26"/>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="25"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="70" t="s">
+        <v>95</v>
+      </c>
+      <c r="G11" s="70"/>
+      <c r="H11" s="71" t="s">
+        <v>64</v>
+      </c>
+      <c r="I11" s="71"/>
+      <c r="J11" s="71"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="26"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="25"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="63" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" s="65"/>
+      <c r="H12" s="72" t="s">
+        <v>97</v>
+      </c>
+      <c r="I12" s="73"/>
+      <c r="J12" s="74"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="26"/>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="25"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="26"/>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="25"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="70" t="s">
+        <v>95</v>
+      </c>
+      <c r="G14" s="70"/>
+      <c r="H14" s="71" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14" s="71"/>
+      <c r="J14" s="71"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="26"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="25"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="63" t="s">
+        <v>175</v>
+      </c>
+      <c r="G15" s="65"/>
+      <c r="H15" s="72" t="s">
+        <v>176</v>
+      </c>
+      <c r="I15" s="73"/>
+      <c r="J15" s="74"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="26"/>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="25"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="26"/>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" s="25"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="26"/>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" s="25"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="58" t="s">
+        <v>65</v>
+      </c>
+      <c r="H18" s="58"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="K18" s="58"/>
+      <c r="L18" s="58"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="26"/>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" s="25"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="H19" s="62"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="66" t="s">
+        <v>72</v>
+      </c>
+      <c r="K19" s="66"/>
+      <c r="L19" s="66"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="22"/>
+      <c r="P19" s="26"/>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" s="25"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="58" t="s">
+        <v>168</v>
+      </c>
+      <c r="I20" s="58"/>
+      <c r="J20" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="K20" s="58"/>
+      <c r="L20" s="58"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="26"/>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" s="25"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="75" t="s">
+        <v>171</v>
+      </c>
+      <c r="I21" s="76"/>
+      <c r="J21" s="66" t="s">
+        <v>169</v>
+      </c>
+      <c r="K21" s="66"/>
+      <c r="L21" s="66"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="22"/>
+      <c r="P21" s="26"/>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" s="31"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="34"/>
+      <c r="O22" s="34"/>
+      <c r="P22" s="36"/>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" s="17"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="17"/>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" s="39"/>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" s="39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="26">
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="K5:P5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:J6"/>
+    <mergeCell ref="K6:P6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P26"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.88671875" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="3" width="3.88671875" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="39"/>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58" t="s">
+        <v>62</v>
+      </c>
+      <c r="L5" s="58"/>
+      <c r="M5" s="58"/>
+      <c r="N5" s="58"/>
+      <c r="O5" s="58"/>
+      <c r="P5" s="58"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="59" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="59" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="L6" s="60"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="60"/>
+      <c r="O6" s="60"/>
+      <c r="P6" s="61"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="20"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="24"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="25"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="67" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="68"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="58" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="58"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="26"/>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="25"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="64"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="66" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" s="66"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="66"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="26"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="25"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="26"/>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="25"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="70" t="s">
+        <v>95</v>
+      </c>
+      <c r="G11" s="70"/>
+      <c r="H11" s="71" t="s">
+        <v>64</v>
+      </c>
+      <c r="I11" s="71"/>
+      <c r="J11" s="71"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="26"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="25"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="63" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" s="65"/>
+      <c r="H12" s="72" t="s">
+        <v>97</v>
+      </c>
+      <c r="I12" s="73"/>
+      <c r="J12" s="74"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="26"/>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="25"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="26"/>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="25"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="70" t="s">
+        <v>95</v>
+      </c>
+      <c r="G14" s="70"/>
+      <c r="H14" s="71" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14" s="71"/>
+      <c r="J14" s="71"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="26"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="25"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="63" t="s">
+        <v>175</v>
+      </c>
+      <c r="G15" s="65"/>
+      <c r="H15" s="72" t="s">
+        <v>176</v>
+      </c>
+      <c r="I15" s="73"/>
+      <c r="J15" s="74"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="26"/>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="25"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="26"/>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" s="25"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="26"/>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" s="25"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="58" t="s">
+        <v>65</v>
+      </c>
+      <c r="H18" s="58"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="K18" s="58"/>
+      <c r="L18" s="58"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="26"/>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" s="25"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="H19" s="62"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="66" t="s">
+        <v>72</v>
+      </c>
+      <c r="K19" s="66"/>
+      <c r="L19" s="66"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="22"/>
+      <c r="P19" s="26"/>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" s="25"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="58" t="s">
+        <v>168</v>
+      </c>
+      <c r="I20" s="58"/>
+      <c r="J20" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="K20" s="58"/>
+      <c r="L20" s="58"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="26"/>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" s="25"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="75" t="s">
+        <v>171</v>
+      </c>
+      <c r="I21" s="76"/>
+      <c r="J21" s="66" t="s">
+        <v>169</v>
+      </c>
+      <c r="K21" s="66"/>
+      <c r="L21" s="66"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="22"/>
+      <c r="P21" s="26"/>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" s="31"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="34"/>
+      <c r="O22" s="34"/>
+      <c r="P22" s="36"/>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" s="17"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="17"/>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" s="39"/>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" s="39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="26">
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="K5:P5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:J6"/>
+    <mergeCell ref="K6:P6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="15.75"/>
@@ -2190,7 +3171,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2198,68 +3179,64 @@
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>76</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>92</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
-        <v>94</v>
+        <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="1"/>
+        <v>174</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E7" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2267,52 +3244,278 @@
         <v>94</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
-        <v>0</v>
+        <v>94</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>167</v>
+        <v>99</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3" t="s">
-        <v>94</v>
+        <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="3"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="A11" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>170</v>
+      </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2322,12 +3525,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S153"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1"/>
@@ -9111,2139 +10314,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q208"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="3.88671875" defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="3" width="3.88671875" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="39"/>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="Q4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="64" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64" t="s">
-        <v>61</v>
-      </c>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="64"/>
-      <c r="J5" s="64"/>
-      <c r="K5" s="64" t="s">
-        <v>62</v>
-      </c>
-      <c r="L5" s="64"/>
-      <c r="M5" s="64"/>
-      <c r="N5" s="64"/>
-      <c r="O5" s="64"/>
-      <c r="P5" s="64"/>
-      <c r="Q5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="A6" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="67" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="67" t="s">
-        <v>74</v>
-      </c>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="69"/>
-      <c r="K6" s="67" t="s">
-        <v>75</v>
-      </c>
-      <c r="L6" s="68"/>
-      <c r="M6" s="68"/>
-      <c r="N6" s="68"/>
-      <c r="O6" s="68"/>
-      <c r="P6" s="69"/>
-      <c r="Q6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
-      <c r="A7" s="20"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="24"/>
-      <c r="Q7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="A8" s="25"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="61" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" s="62"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="64" t="s">
-        <v>64</v>
-      </c>
-      <c r="H8" s="64"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="64"/>
-      <c r="K8" s="64"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="26"/>
-      <c r="Q8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
-      <c r="A9" s="25"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="71" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9" s="72"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="74" t="s">
-        <v>70</v>
-      </c>
-      <c r="H9" s="74"/>
-      <c r="I9" s="74"/>
-      <c r="J9" s="74"/>
-      <c r="K9" s="74"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="26"/>
-      <c r="Q9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
-      <c r="A10" s="25"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="46"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="26"/>
-      <c r="Q10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="A11" s="25"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="75" t="s">
-        <v>95</v>
-      </c>
-      <c r="G11" s="75"/>
-      <c r="H11" s="76" t="s">
-        <v>64</v>
-      </c>
-      <c r="I11" s="76"/>
-      <c r="J11" s="76"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="26"/>
-      <c r="Q11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
-      <c r="A12" s="25"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="71" t="s">
-        <v>96</v>
-      </c>
-      <c r="G12" s="73"/>
-      <c r="H12" s="77" t="s">
-        <v>97</v>
-      </c>
-      <c r="I12" s="78"/>
-      <c r="J12" s="79"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="26"/>
-      <c r="Q12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
-      <c r="A13" s="25"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="71" t="s">
-        <v>96</v>
-      </c>
-      <c r="G13" s="73"/>
-      <c r="H13" s="77" t="s">
-        <v>97</v>
-      </c>
-      <c r="I13" s="78"/>
-      <c r="J13" s="79"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="26"/>
-      <c r="Q13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
-      <c r="A14" s="25"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="26"/>
-      <c r="Q14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
-      <c r="A15" s="25"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="75" t="s">
-        <v>95</v>
-      </c>
-      <c r="G15" s="75"/>
-      <c r="H15" s="76" t="s">
-        <v>64</v>
-      </c>
-      <c r="I15" s="76"/>
-      <c r="J15" s="76"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="26"/>
-      <c r="Q15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
-      <c r="A16" s="25"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="71" t="s">
-        <v>96</v>
-      </c>
-      <c r="G16" s="73"/>
-      <c r="H16" s="77" t="s">
-        <v>97</v>
-      </c>
-      <c r="I16" s="78"/>
-      <c r="J16" s="79"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="26"/>
-      <c r="Q16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
-      <c r="A17" s="25"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="71" t="s">
-        <v>96</v>
-      </c>
-      <c r="G17" s="73"/>
-      <c r="H17" s="77" t="s">
-        <v>97</v>
-      </c>
-      <c r="I17" s="78"/>
-      <c r="J17" s="79"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="26"/>
-      <c r="Q17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17">
-      <c r="A18" s="25"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="48"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="36"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="23"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="26"/>
-      <c r="Q18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
-      <c r="A19" s="25"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="71" t="s">
-        <v>69</v>
-      </c>
-      <c r="E19" s="72"/>
-      <c r="F19" s="73"/>
-      <c r="G19" s="74" t="s">
-        <v>70</v>
-      </c>
-      <c r="H19" s="74"/>
-      <c r="I19" s="74"/>
-      <c r="J19" s="74"/>
-      <c r="K19" s="74"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="26"/>
-      <c r="Q19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17">
-      <c r="A20" s="25"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="46"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="23"/>
-      <c r="O20" s="23"/>
-      <c r="P20" s="26"/>
-      <c r="Q20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17">
-      <c r="A21" s="25"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="75" t="s">
-        <v>95</v>
-      </c>
-      <c r="G21" s="75"/>
-      <c r="H21" s="76" t="s">
-        <v>64</v>
-      </c>
-      <c r="I21" s="76"/>
-      <c r="J21" s="76"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="23"/>
-      <c r="N21" s="23"/>
-      <c r="O21" s="23"/>
-      <c r="P21" s="26"/>
-      <c r="Q21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17">
-      <c r="A22" s="25"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="71" t="s">
-        <v>96</v>
-      </c>
-      <c r="G22" s="73"/>
-      <c r="H22" s="77" t="s">
-        <v>97</v>
-      </c>
-      <c r="I22" s="78"/>
-      <c r="J22" s="79"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
-      <c r="N22" s="23"/>
-      <c r="O22" s="23"/>
-      <c r="P22" s="26"/>
-      <c r="Q22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17">
-      <c r="A23" s="25"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="71" t="s">
-        <v>96</v>
-      </c>
-      <c r="G23" s="73"/>
-      <c r="H23" s="77" t="s">
-        <v>97</v>
-      </c>
-      <c r="I23" s="78"/>
-      <c r="J23" s="79"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="23"/>
-      <c r="O23" s="23"/>
-      <c r="P23" s="26"/>
-      <c r="Q23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17">
-      <c r="A24" s="25"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="23"/>
-      <c r="M24" s="23"/>
-      <c r="N24" s="23"/>
-      <c r="O24" s="23"/>
-      <c r="P24" s="26"/>
-      <c r="Q24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17">
-      <c r="A25" s="25"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="75" t="s">
-        <v>95</v>
-      </c>
-      <c r="G25" s="75"/>
-      <c r="H25" s="76" t="s">
-        <v>64</v>
-      </c>
-      <c r="I25" s="76"/>
-      <c r="J25" s="76"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="23"/>
-      <c r="M25" s="23"/>
-      <c r="N25" s="23"/>
-      <c r="O25" s="23"/>
-      <c r="P25" s="26"/>
-      <c r="Q25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17">
-      <c r="A26" s="25"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="71" t="s">
-        <v>96</v>
-      </c>
-      <c r="G26" s="73"/>
-      <c r="H26" s="77" t="s">
-        <v>97</v>
-      </c>
-      <c r="I26" s="78"/>
-      <c r="J26" s="79"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="23"/>
-      <c r="N26" s="23"/>
-      <c r="O26" s="23"/>
-      <c r="P26" s="26"/>
-      <c r="Q26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17">
-      <c r="A27" s="25"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="49"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="71" t="s">
-        <v>96</v>
-      </c>
-      <c r="G27" s="73"/>
-      <c r="H27" s="77" t="s">
-        <v>97</v>
-      </c>
-      <c r="I27" s="78"/>
-      <c r="J27" s="79"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="23"/>
-      <c r="M27" s="23"/>
-      <c r="N27" s="23"/>
-      <c r="O27" s="23"/>
-      <c r="P27" s="26"/>
-      <c r="Q27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17">
-      <c r="A28" s="25"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="48"/>
-      <c r="H28" s="48"/>
-      <c r="I28" s="48"/>
-      <c r="J28" s="34"/>
-      <c r="K28" s="36"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="23"/>
-      <c r="P28" s="26"/>
-      <c r="Q28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17">
-      <c r="A29" s="25"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" s="71" t="s">
-        <v>69</v>
-      </c>
-      <c r="E29" s="72"/>
-      <c r="F29" s="73"/>
-      <c r="G29" s="74" t="s">
-        <v>70</v>
-      </c>
-      <c r="H29" s="74"/>
-      <c r="I29" s="74"/>
-      <c r="J29" s="74"/>
-      <c r="K29" s="74"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
-      <c r="P29" s="26"/>
-      <c r="Q29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17">
-      <c r="A30" s="25"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="46"/>
-      <c r="K30" s="24"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="23"/>
-      <c r="N30" s="23"/>
-      <c r="O30" s="23"/>
-      <c r="P30" s="26"/>
-      <c r="Q30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="A31" s="25"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="49"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="75" t="s">
-        <v>95</v>
-      </c>
-      <c r="G31" s="75"/>
-      <c r="H31" s="76" t="s">
-        <v>64</v>
-      </c>
-      <c r="I31" s="76"/>
-      <c r="J31" s="76"/>
-      <c r="K31" s="26"/>
-      <c r="L31" s="23"/>
-      <c r="M31" s="23"/>
-      <c r="N31" s="23"/>
-      <c r="O31" s="23"/>
-      <c r="P31" s="26"/>
-      <c r="Q31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17">
-      <c r="A32" s="25"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="49"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="71" t="s">
-        <v>96</v>
-      </c>
-      <c r="G32" s="73"/>
-      <c r="H32" s="77" t="s">
-        <v>97</v>
-      </c>
-      <c r="I32" s="78"/>
-      <c r="J32" s="79"/>
-      <c r="K32" s="26"/>
-      <c r="L32" s="23"/>
-      <c r="M32" s="23"/>
-      <c r="N32" s="23"/>
-      <c r="O32" s="23"/>
-      <c r="P32" s="26"/>
-      <c r="Q32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17">
-      <c r="A33" s="25"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="49"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="71" t="s">
-        <v>96</v>
-      </c>
-      <c r="G33" s="73"/>
-      <c r="H33" s="77" t="s">
-        <v>97</v>
-      </c>
-      <c r="I33" s="78"/>
-      <c r="J33" s="79"/>
-      <c r="K33" s="26"/>
-      <c r="L33" s="23"/>
-      <c r="M33" s="23"/>
-      <c r="N33" s="23"/>
-      <c r="O33" s="23"/>
-      <c r="P33" s="26"/>
-      <c r="Q33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17">
-      <c r="A34" s="25"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="49"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="42"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="43"/>
-      <c r="I34" s="43"/>
-      <c r="J34" s="22"/>
-      <c r="K34" s="26"/>
-      <c r="L34" s="23"/>
-      <c r="M34" s="23"/>
-      <c r="N34" s="23"/>
-      <c r="O34" s="23"/>
-      <c r="P34" s="26"/>
-      <c r="Q34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17">
-      <c r="A35" s="25"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="75" t="s">
-        <v>95</v>
-      </c>
-      <c r="G35" s="75"/>
-      <c r="H35" s="76" t="s">
-        <v>64</v>
-      </c>
-      <c r="I35" s="76"/>
-      <c r="J35" s="76"/>
-      <c r="K35" s="26"/>
-      <c r="L35" s="23"/>
-      <c r="M35" s="23"/>
-      <c r="N35" s="23"/>
-      <c r="O35" s="23"/>
-      <c r="P35" s="26"/>
-      <c r="Q35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17">
-      <c r="A36" s="25"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="71" t="s">
-        <v>96</v>
-      </c>
-      <c r="G36" s="73"/>
-      <c r="H36" s="77" t="s">
-        <v>97</v>
-      </c>
-      <c r="I36" s="78"/>
-      <c r="J36" s="79"/>
-      <c r="K36" s="26"/>
-      <c r="L36" s="23"/>
-      <c r="M36" s="23"/>
-      <c r="N36" s="23"/>
-      <c r="O36" s="23"/>
-      <c r="P36" s="26"/>
-      <c r="Q36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17">
-      <c r="A37" s="25"/>
-      <c r="B37" s="21"/>
-      <c r="C37" s="49"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="71" t="s">
-        <v>96</v>
-      </c>
-      <c r="G37" s="73"/>
-      <c r="H37" s="77" t="s">
-        <v>97</v>
-      </c>
-      <c r="I37" s="78"/>
-      <c r="J37" s="79"/>
-      <c r="K37" s="26"/>
-      <c r="L37" s="23"/>
-      <c r="M37" s="23"/>
-      <c r="N37" s="23"/>
-      <c r="O37" s="23"/>
-      <c r="P37" s="26"/>
-      <c r="Q37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17">
-      <c r="A38" s="25"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="50"/>
-      <c r="D38" s="47"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="48"/>
-      <c r="H38" s="48"/>
-      <c r="I38" s="48"/>
-      <c r="J38" s="34"/>
-      <c r="K38" s="36"/>
-      <c r="L38" s="23"/>
-      <c r="M38" s="23"/>
-      <c r="N38" s="23"/>
-      <c r="O38" s="23"/>
-      <c r="P38" s="26"/>
-      <c r="Q38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17">
-      <c r="A39" s="25"/>
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="22"/>
-      <c r="J39" s="22"/>
-      <c r="K39" s="23"/>
-      <c r="L39" s="23"/>
-      <c r="M39" s="23"/>
-      <c r="N39" s="23"/>
-      <c r="O39" s="23"/>
-      <c r="P39" s="26"/>
-      <c r="Q39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17">
-      <c r="A40" s="25"/>
-      <c r="B40" s="21"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="G40" s="64" t="s">
-        <v>65</v>
-      </c>
-      <c r="H40" s="64"/>
-      <c r="I40" s="64"/>
-      <c r="J40" s="64" t="s">
-        <v>66</v>
-      </c>
-      <c r="K40" s="64"/>
-      <c r="L40" s="64"/>
-      <c r="M40" s="23"/>
-      <c r="N40" s="23"/>
-      <c r="O40" s="23"/>
-      <c r="P40" s="26"/>
-      <c r="Q40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17">
-      <c r="A41" s="25"/>
-      <c r="B41" s="21"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="G41" s="70" t="s">
-        <v>71</v>
-      </c>
-      <c r="H41" s="70"/>
-      <c r="I41" s="70"/>
-      <c r="J41" s="74" t="s">
-        <v>72</v>
-      </c>
-      <c r="K41" s="74"/>
-      <c r="L41" s="74"/>
-      <c r="M41" s="22"/>
-      <c r="N41" s="22"/>
-      <c r="O41" s="22"/>
-      <c r="P41" s="26"/>
-      <c r="Q41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17">
-      <c r="A42" s="25"/>
-      <c r="B42" s="21"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="54"/>
-      <c r="G42" s="53"/>
-      <c r="H42" s="64" t="s">
-        <v>168</v>
-      </c>
-      <c r="I42" s="64"/>
-      <c r="J42" s="64" t="s">
-        <v>66</v>
-      </c>
-      <c r="K42" s="64"/>
-      <c r="L42" s="64"/>
-      <c r="M42" s="22"/>
-      <c r="N42" s="22"/>
-      <c r="O42" s="22"/>
-      <c r="P42" s="26"/>
-      <c r="Q42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17">
-      <c r="A43" s="25"/>
-      <c r="B43" s="21"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="55"/>
-      <c r="G43" s="34"/>
-      <c r="H43" s="80" t="s">
-        <v>171</v>
-      </c>
-      <c r="I43" s="81"/>
-      <c r="J43" s="74" t="s">
-        <v>169</v>
-      </c>
-      <c r="K43" s="74"/>
-      <c r="L43" s="74"/>
-      <c r="M43" s="22"/>
-      <c r="N43" s="22"/>
-      <c r="O43" s="22"/>
-      <c r="P43" s="26"/>
-      <c r="Q43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17">
-      <c r="A44" s="25"/>
-      <c r="B44" s="21"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="55"/>
-      <c r="G44" s="34"/>
-      <c r="H44" s="80" t="s">
-        <v>171</v>
-      </c>
-      <c r="I44" s="81"/>
-      <c r="J44" s="74" t="s">
-        <v>169</v>
-      </c>
-      <c r="K44" s="74"/>
-      <c r="L44" s="74"/>
-      <c r="M44" s="22"/>
-      <c r="N44" s="22"/>
-      <c r="O44" s="22"/>
-      <c r="P44" s="26"/>
-      <c r="Q44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17">
-      <c r="A45" s="25"/>
-      <c r="B45" s="21"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="22"/>
-      <c r="E45" s="22"/>
-      <c r="F45" s="55"/>
-      <c r="G45" s="34"/>
-      <c r="H45" s="80" t="s">
-        <v>171</v>
-      </c>
-      <c r="I45" s="81"/>
-      <c r="J45" s="74" t="s">
-        <v>169</v>
-      </c>
-      <c r="K45" s="74"/>
-      <c r="L45" s="74"/>
-      <c r="M45" s="22"/>
-      <c r="N45" s="22"/>
-      <c r="O45" s="22"/>
-      <c r="P45" s="26"/>
-      <c r="Q45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17">
-      <c r="A46" s="25"/>
-      <c r="B46" s="21"/>
-      <c r="C46" s="30"/>
-      <c r="D46" s="22"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="G46" s="70" t="s">
-        <v>71</v>
-      </c>
-      <c r="H46" s="70"/>
-      <c r="I46" s="70"/>
-      <c r="J46" s="74" t="s">
-        <v>72</v>
-      </c>
-      <c r="K46" s="74"/>
-      <c r="L46" s="74"/>
-      <c r="M46" s="22"/>
-      <c r="N46" s="22"/>
-      <c r="O46" s="22"/>
-      <c r="P46" s="26"/>
-      <c r="Q46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17">
-      <c r="A47" s="25"/>
-      <c r="B47" s="21"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="22"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="54"/>
-      <c r="G47" s="53"/>
-      <c r="H47" s="64" t="s">
-        <v>168</v>
-      </c>
-      <c r="I47" s="64"/>
-      <c r="J47" s="64" t="s">
-        <v>66</v>
-      </c>
-      <c r="K47" s="64"/>
-      <c r="L47" s="64"/>
-      <c r="M47" s="22"/>
-      <c r="N47" s="22"/>
-      <c r="O47" s="22"/>
-      <c r="P47" s="26"/>
-      <c r="Q47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17">
-      <c r="A48" s="25"/>
-      <c r="B48" s="21"/>
-      <c r="C48" s="30"/>
-      <c r="D48" s="22"/>
-      <c r="E48" s="22"/>
-      <c r="F48" s="55"/>
-      <c r="G48" s="34"/>
-      <c r="H48" s="80" t="s">
-        <v>171</v>
-      </c>
-      <c r="I48" s="81"/>
-      <c r="J48" s="74" t="s">
-        <v>169</v>
-      </c>
-      <c r="K48" s="74"/>
-      <c r="L48" s="74"/>
-      <c r="M48" s="22"/>
-      <c r="N48" s="22"/>
-      <c r="O48" s="22"/>
-      <c r="P48" s="26"/>
-      <c r="Q48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17">
-      <c r="A49" s="25"/>
-      <c r="B49" s="21"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="22"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="55"/>
-      <c r="G49" s="34"/>
-      <c r="H49" s="80" t="s">
-        <v>171</v>
-      </c>
-      <c r="I49" s="81"/>
-      <c r="J49" s="74" t="s">
-        <v>169</v>
-      </c>
-      <c r="K49" s="74"/>
-      <c r="L49" s="74"/>
-      <c r="M49" s="22"/>
-      <c r="N49" s="22"/>
-      <c r="O49" s="22"/>
-      <c r="P49" s="26"/>
-      <c r="Q49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17">
-      <c r="A50" s="25"/>
-      <c r="B50" s="21"/>
-      <c r="C50" s="30"/>
-      <c r="D50" s="22"/>
-      <c r="E50" s="22"/>
-      <c r="F50" s="55"/>
-      <c r="G50" s="34"/>
-      <c r="H50" s="80" t="s">
-        <v>171</v>
-      </c>
-      <c r="I50" s="81"/>
-      <c r="J50" s="74" t="s">
-        <v>169</v>
-      </c>
-      <c r="K50" s="74"/>
-      <c r="L50" s="74"/>
-      <c r="M50" s="22"/>
-      <c r="N50" s="22"/>
-      <c r="O50" s="22"/>
-      <c r="P50" s="26"/>
-      <c r="Q50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17">
-      <c r="A51" s="31"/>
-      <c r="B51" s="32"/>
-      <c r="C51" s="33"/>
-      <c r="D51" s="34"/>
-      <c r="E51" s="34"/>
-      <c r="F51" s="35"/>
-      <c r="G51" s="35"/>
-      <c r="H51" s="35"/>
-      <c r="I51" s="35"/>
-      <c r="J51" s="35"/>
-      <c r="K51" s="35"/>
-      <c r="L51" s="35"/>
-      <c r="M51" s="34"/>
-      <c r="N51" s="34"/>
-      <c r="O51" s="34"/>
-      <c r="P51" s="36"/>
-      <c r="Q51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17">
-      <c r="A52" s="28"/>
-      <c r="B52" s="21"/>
-      <c r="C52" s="30"/>
-      <c r="D52" s="22"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="56"/>
-      <c r="G52" s="56"/>
-      <c r="H52" s="56"/>
-      <c r="I52" s="56"/>
-      <c r="J52" s="56"/>
-      <c r="K52" s="56"/>
-      <c r="L52" s="56"/>
-      <c r="M52" s="22"/>
-      <c r="N52" s="22"/>
-      <c r="O52" s="22"/>
-      <c r="P52" s="22"/>
-      <c r="Q52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17">
-      <c r="A53" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="B53" s="61" t="s">
-        <v>63</v>
-      </c>
-      <c r="C53" s="62"/>
-      <c r="D53" s="63"/>
-      <c r="E53" s="64" t="s">
-        <v>64</v>
-      </c>
-      <c r="F53" s="64"/>
-      <c r="G53" s="64"/>
-      <c r="H53" s="64"/>
-      <c r="I53" s="64"/>
-      <c r="J53" s="56"/>
-      <c r="K53" s="56"/>
-      <c r="L53" s="56"/>
-      <c r="M53" s="22"/>
-      <c r="N53" s="22"/>
-      <c r="O53" s="22"/>
-      <c r="P53" s="22"/>
-      <c r="Q53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17">
-      <c r="A54" s="57"/>
-      <c r="B54" s="66"/>
-      <c r="C54" s="66"/>
-      <c r="D54" s="66"/>
-      <c r="E54" s="65"/>
-      <c r="F54" s="65"/>
-      <c r="G54" s="65"/>
-      <c r="H54" s="65"/>
-      <c r="I54" s="65"/>
-      <c r="J54" s="56"/>
-      <c r="K54" s="56"/>
-      <c r="L54" s="56"/>
-      <c r="M54" s="22"/>
-      <c r="N54" s="22"/>
-      <c r="O54" s="22"/>
-      <c r="P54" s="22"/>
-      <c r="Q54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17">
-      <c r="A55" s="17"/>
-      <c r="B55" s="18"/>
-      <c r="C55" s="18"/>
-      <c r="D55" s="17"/>
-      <c r="Q55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17">
-      <c r="A56" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17">
-      <c r="A57" s="39"/>
-      <c r="Q57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17">
-      <c r="A58" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17">
-      <c r="Q59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17">
-      <c r="Q60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17">
-      <c r="Q61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17">
-      <c r="Q62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17">
-      <c r="Q63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17">
-      <c r="Q64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="17:17">
-      <c r="Q65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="17:17">
-      <c r="Q66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="17:17">
-      <c r="Q67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="17:17">
-      <c r="Q68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="17:17">
-      <c r="Q69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="17:17">
-      <c r="Q70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="17:17">
-      <c r="Q71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="17:17">
-      <c r="Q72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="17:17">
-      <c r="Q73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="17:17">
-      <c r="Q74">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="17:17">
-      <c r="Q75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="17:17">
-      <c r="Q76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="17:17">
-      <c r="Q77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="17:17">
-      <c r="Q78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="17:17">
-      <c r="Q79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="17:17">
-      <c r="Q80">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="17:17">
-      <c r="Q81">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="17:17">
-      <c r="Q82">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="17:17">
-      <c r="Q83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="17:17">
-      <c r="Q84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="17:17">
-      <c r="Q85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="17:17">
-      <c r="Q86">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="17:17">
-      <c r="Q87">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="17:17">
-      <c r="Q88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="17:17">
-      <c r="Q89">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="17:17">
-      <c r="Q90">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="17:17">
-      <c r="Q91">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="17:17">
-      <c r="Q92">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="17:17">
-      <c r="Q93">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="17:17">
-      <c r="Q94">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="17:17">
-      <c r="Q95">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="17:17">
-      <c r="Q96">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="17:17">
-      <c r="Q97">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="17:17">
-      <c r="Q98">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="17:17">
-      <c r="Q99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="17:17">
-      <c r="Q100">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="17:17">
-      <c r="Q101">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="17:17">
-      <c r="Q102">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="17:17">
-      <c r="Q103">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="17:17">
-      <c r="Q104">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="17:17">
-      <c r="Q105">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="17:17">
-      <c r="Q106">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="17:17">
-      <c r="Q107">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="17:17">
-      <c r="Q108">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="17:17">
-      <c r="Q109">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="110" spans="17:17">
-      <c r="Q110">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="111" spans="17:17">
-      <c r="Q111">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112" spans="17:17">
-      <c r="Q112">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113" spans="17:17">
-      <c r="Q113">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="114" spans="17:17">
-      <c r="Q114">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="115" spans="17:17">
-      <c r="Q115">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="116" spans="17:17">
-      <c r="Q116">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117" spans="17:17">
-      <c r="Q117">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="17:17">
-      <c r="Q118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119" spans="17:17">
-      <c r="Q119">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="17:17">
-      <c r="Q120">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121" spans="17:17">
-      <c r="Q121">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122" spans="17:17">
-      <c r="Q122">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="123" spans="17:17">
-      <c r="Q123">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124" spans="17:17">
-      <c r="Q124">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="125" spans="17:17">
-      <c r="Q125">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="126" spans="17:17">
-      <c r="Q126">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="127" spans="17:17">
-      <c r="Q127">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="128" spans="17:17">
-      <c r="Q128">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="129" spans="17:17">
-      <c r="Q129">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="130" spans="17:17">
-      <c r="Q130">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="131" spans="17:17">
-      <c r="Q131">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="132" spans="17:17">
-      <c r="Q132">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="133" spans="17:17">
-      <c r="Q133">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="134" spans="17:17">
-      <c r="Q134">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="135" spans="17:17">
-      <c r="Q135">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="136" spans="17:17">
-      <c r="Q136">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="17:17">
-      <c r="Q137">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="138" spans="17:17">
-      <c r="Q138">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="139" spans="17:17">
-      <c r="Q139">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="140" spans="17:17">
-      <c r="Q140">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="141" spans="17:17">
-      <c r="Q141">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="17:17">
-      <c r="Q142">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="17:17">
-      <c r="Q143">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144" spans="17:17">
-      <c r="Q144">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="145" spans="17:17">
-      <c r="Q145">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="146" spans="17:17">
-      <c r="Q146">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="147" spans="17:17">
-      <c r="Q147">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="148" spans="17:17">
-      <c r="Q148">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="149" spans="17:17">
-      <c r="Q149">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="150" spans="17:17">
-      <c r="Q150">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="151" spans="17:17">
-      <c r="Q151">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="152" spans="17:17">
-      <c r="Q152">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="153" spans="17:17">
-      <c r="Q153">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="154" spans="17:17">
-      <c r="Q154">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="155" spans="17:17">
-      <c r="Q155">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="156" spans="17:17">
-      <c r="Q156">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="157" spans="17:17">
-      <c r="Q157">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="158" spans="17:17">
-      <c r="Q158">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="159" spans="17:17">
-      <c r="Q159">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="160" spans="17:17">
-      <c r="Q160">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="161" spans="17:17">
-      <c r="Q161">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="162" spans="17:17">
-      <c r="Q162">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="163" spans="17:17">
-      <c r="Q163">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="164" spans="17:17">
-      <c r="Q164">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="165" spans="17:17">
-      <c r="Q165">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="166" spans="17:17">
-      <c r="Q166">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="167" spans="17:17">
-      <c r="Q167">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="168" spans="17:17">
-      <c r="Q168">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="169" spans="17:17">
-      <c r="Q169">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="170" spans="17:17">
-      <c r="Q170">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="171" spans="17:17">
-      <c r="Q171">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="172" spans="17:17">
-      <c r="Q172">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="173" spans="17:17">
-      <c r="Q173">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="174" spans="17:17">
-      <c r="Q174">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="175" spans="17:17">
-      <c r="Q175">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="176" spans="17:17">
-      <c r="Q176">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="177" spans="17:17">
-      <c r="Q177">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="178" spans="17:17">
-      <c r="Q178">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="179" spans="17:17">
-      <c r="Q179">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="180" spans="17:17">
-      <c r="Q180">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="181" spans="17:17">
-      <c r="Q181">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="182" spans="17:17">
-      <c r="Q182">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="183" spans="17:17">
-      <c r="Q183">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="184" spans="17:17">
-      <c r="Q184">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="185" spans="17:17">
-      <c r="Q185">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="186" spans="17:17">
-      <c r="Q186">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="187" spans="17:17">
-      <c r="Q187">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="188" spans="17:17">
-      <c r="Q188">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="189" spans="17:17">
-      <c r="Q189">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="190" spans="17:17">
-      <c r="Q190">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="191" spans="17:17">
-      <c r="Q191">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="192" spans="17:17">
-      <c r="Q192">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="193" spans="17:17">
-      <c r="Q193">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="194" spans="17:17">
-      <c r="Q194">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="195" spans="17:17">
-      <c r="Q195">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="196" spans="17:17">
-      <c r="Q196">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="197" spans="17:17">
-      <c r="Q197">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="198" spans="17:17">
-      <c r="Q198">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="199" spans="17:17">
-      <c r="Q199">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="200" spans="17:17">
-      <c r="Q200">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="201" spans="17:17">
-      <c r="Q201">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="202" spans="17:17">
-      <c r="Q202">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="203" spans="17:17">
-      <c r="Q203">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="204" spans="17:17">
-      <c r="Q204">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="205" spans="17:17">
-      <c r="Q205">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="206" spans="17:17">
-      <c r="Q206">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="207" spans="17:17">
-      <c r="Q207">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="208" spans="17:17">
-      <c r="Q208">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="76">
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F5:J5"/>
-    <mergeCell ref="K5:P5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:J6"/>
-    <mergeCell ref="K6:P6"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="H37:J37"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="G29:K29"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="H31:J31"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H32:J32"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="J40:L40"/>
-    <mergeCell ref="G46:I46"/>
-    <mergeCell ref="J46:L46"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="J47:L47"/>
-    <mergeCell ref="G41:I41"/>
-    <mergeCell ref="J41:L41"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="J42:L42"/>
-    <mergeCell ref="J45:L45"/>
-    <mergeCell ref="J43:L43"/>
-    <mergeCell ref="J44:L44"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="E53:I53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="E54:I54"/>
-    <mergeCell ref="G40:I40"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="J48:L48"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="J49:L49"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="J50:L50"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="H33:J33"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="H35:J35"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="G19:K19"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:J25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:J27"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>